<commit_message>
Updated final for thesis
</commit_message>
<xml_diff>
--- a/Phase 2/Comparison with VTO/Detailed analysis/WEB_scenario_3/web_all_vto_common_WEB_JEFF_shrtlist_200308_rel_over10.xlsx
+++ b/Phase 2/Comparison with VTO/Detailed analysis/WEB_scenario_3/web_all_vto_common_WEB_JEFF_shrtlist_200308_rel_over10.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Documents\GitHub\Appendices\Phase 2\Comparison with VTO\Detailed analysis\WEB_scenario_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88FE4DE7-0368-4F7F-B67F-69DEA7ECD040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7382728F-1F6F-486E-A333-D8E9A59D3D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web_all_vto_common_WEB_JEFF_shr" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="308">
   <si>
     <t>TAXRANK_target</t>
   </si>
@@ -950,7 +950,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1784,11 +1784,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I175"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139:I175"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,10 +2929,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2944,7 +2944,7 @@
         <v>14</v>
       </c>
       <c r="G40">
-        <v>11.83</v>
+        <v>13.66</v>
       </c>
       <c r="H40" t="s">
         <v>15</v>
@@ -2958,10 +2958,10 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2973,7 +2973,7 @@
         <v>14</v>
       </c>
       <c r="G41">
-        <v>13.66</v>
+        <v>13.08</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -2987,7 +2987,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
         <v>74</v>
@@ -3002,7 +3002,7 @@
         <v>14</v>
       </c>
       <c r="G42">
-        <v>13.08</v>
+        <v>13.03</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -3016,10 +3016,10 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -3031,7 +3031,7 @@
         <v>14</v>
       </c>
       <c r="G43">
-        <v>13.03</v>
+        <v>13.96</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -3045,10 +3045,10 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -3060,7 +3060,7 @@
         <v>14</v>
       </c>
       <c r="G44">
-        <v>13.96</v>
+        <v>13.89</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -3074,10 +3074,10 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -3089,7 +3089,7 @@
         <v>14</v>
       </c>
       <c r="G45">
-        <v>13.89</v>
+        <v>12.79</v>
       </c>
       <c r="H45" t="s">
         <v>15</v>
@@ -3103,10 +3103,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3118,7 +3118,7 @@
         <v>14</v>
       </c>
       <c r="G46">
-        <v>12.79</v>
+        <v>13.94</v>
       </c>
       <c r="H46" t="s">
         <v>15</v>
@@ -3132,10 +3132,10 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -3147,7 +3147,7 @@
         <v>14</v>
       </c>
       <c r="G47">
-        <v>13.94</v>
+        <v>13.97</v>
       </c>
       <c r="H47" t="s">
         <v>15</v>
@@ -3161,10 +3161,10 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -3176,7 +3176,7 @@
         <v>14</v>
       </c>
       <c r="G48">
-        <v>13.97</v>
+        <v>13.9</v>
       </c>
       <c r="H48" t="s">
         <v>15</v>
@@ -3190,10 +3190,10 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
@@ -3205,7 +3205,7 @@
         <v>14</v>
       </c>
       <c r="G49">
-        <v>13.9</v>
+        <v>13.85</v>
       </c>
       <c r="H49" t="s">
         <v>15</v>
@@ -3219,10 +3219,10 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3234,7 +3234,7 @@
         <v>14</v>
       </c>
       <c r="G50">
-        <v>13.85</v>
+        <v>13.41</v>
       </c>
       <c r="H50" t="s">
         <v>15</v>
@@ -3248,10 +3248,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -3263,7 +3263,7 @@
         <v>14</v>
       </c>
       <c r="G51">
-        <v>13.41</v>
+        <v>13.55</v>
       </c>
       <c r="H51" t="s">
         <v>15</v>
@@ -3277,10 +3277,10 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3292,7 +3292,7 @@
         <v>14</v>
       </c>
       <c r="G52">
-        <v>13.55</v>
+        <v>13.94</v>
       </c>
       <c r="H52" t="s">
         <v>15</v>
@@ -3306,10 +3306,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -3321,7 +3321,7 @@
         <v>14</v>
       </c>
       <c r="G53">
-        <v>13.94</v>
+        <v>13.5</v>
       </c>
       <c r="H53" t="s">
         <v>15</v>
@@ -3335,10 +3335,10 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -3350,7 +3350,7 @@
         <v>14</v>
       </c>
       <c r="G54">
-        <v>13.5</v>
+        <v>13.88</v>
       </c>
       <c r="H54" t="s">
         <v>15</v>
@@ -3364,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -3379,7 +3379,7 @@
         <v>14</v>
       </c>
       <c r="G55">
-        <v>13.88</v>
+        <v>12.68</v>
       </c>
       <c r="H55" t="s">
         <v>15</v>
@@ -3393,7 +3393,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
         <v>95</v>
@@ -3408,7 +3408,7 @@
         <v>14</v>
       </c>
       <c r="G56">
-        <v>12.68</v>
+        <v>11.57</v>
       </c>
       <c r="H56" t="s">
         <v>15</v>
@@ -3422,10 +3422,10 @@
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -3437,7 +3437,7 @@
         <v>14</v>
       </c>
       <c r="G57">
-        <v>11.57</v>
+        <v>13.84</v>
       </c>
       <c r="H57" t="s">
         <v>15</v>
@@ -3451,10 +3451,10 @@
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3466,7 +3466,7 @@
         <v>14</v>
       </c>
       <c r="G58">
-        <v>13.84</v>
+        <v>13.62</v>
       </c>
       <c r="H58" t="s">
         <v>15</v>
@@ -3480,10 +3480,10 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -3495,7 +3495,7 @@
         <v>14</v>
       </c>
       <c r="G59">
-        <v>13.62</v>
+        <v>13.32</v>
       </c>
       <c r="H59" t="s">
         <v>15</v>
@@ -3509,7 +3509,7 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -3524,7 +3524,7 @@
         <v>14</v>
       </c>
       <c r="G60">
-        <v>13.32</v>
+        <v>12.97</v>
       </c>
       <c r="H60" t="s">
         <v>15</v>
@@ -3538,10 +3538,10 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -3553,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="G61">
-        <v>12.97</v>
+        <v>13.8</v>
       </c>
       <c r="H61" t="s">
         <v>15</v>
@@ -3567,10 +3567,10 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -3582,7 +3582,7 @@
         <v>14</v>
       </c>
       <c r="G62">
-        <v>13.8</v>
+        <v>12.41</v>
       </c>
       <c r="H62" t="s">
         <v>15</v>
@@ -3596,7 +3596,7 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
         <v>107</v>
@@ -3611,7 +3611,7 @@
         <v>14</v>
       </c>
       <c r="G63">
-        <v>12.41</v>
+        <v>10.73</v>
       </c>
       <c r="H63" t="s">
         <v>15</v>
@@ -3625,10 +3625,10 @@
         <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3640,7 +3640,7 @@
         <v>14</v>
       </c>
       <c r="G64">
-        <v>10.73</v>
+        <v>13.96</v>
       </c>
       <c r="H64" t="s">
         <v>15</v>
@@ -3654,10 +3654,10 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -3669,7 +3669,7 @@
         <v>14</v>
       </c>
       <c r="G65">
-        <v>13.96</v>
+        <v>13.99</v>
       </c>
       <c r="H65" t="s">
         <v>15</v>
@@ -3683,10 +3683,10 @@
         <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C66" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
@@ -3698,7 +3698,7 @@
         <v>14</v>
       </c>
       <c r="G66">
-        <v>13.99</v>
+        <v>13.75</v>
       </c>
       <c r="H66" t="s">
         <v>15</v>
@@ -3712,7 +3712,7 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C67" t="s">
         <v>114</v>
@@ -3727,7 +3727,7 @@
         <v>14</v>
       </c>
       <c r="G67">
-        <v>13.75</v>
+        <v>12.57</v>
       </c>
       <c r="H67" t="s">
         <v>15</v>
@@ -3741,10 +3741,10 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -3756,7 +3756,7 @@
         <v>14</v>
       </c>
       <c r="G68">
-        <v>12.57</v>
+        <v>13.69</v>
       </c>
       <c r="H68" t="s">
         <v>15</v>
@@ -3770,10 +3770,10 @@
         <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -3785,7 +3785,7 @@
         <v>14</v>
       </c>
       <c r="G69">
-        <v>13.69</v>
+        <v>13.57</v>
       </c>
       <c r="H69" t="s">
         <v>15</v>
@@ -3799,7 +3799,7 @@
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C70" t="s">
         <v>119</v>
@@ -3814,7 +3814,7 @@
         <v>14</v>
       </c>
       <c r="G70">
-        <v>13.57</v>
+        <v>13</v>
       </c>
       <c r="H70" t="s">
         <v>15</v>
@@ -3828,10 +3828,10 @@
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
@@ -3843,7 +3843,7 @@
         <v>14</v>
       </c>
       <c r="G71">
-        <v>13</v>
+        <v>11.44</v>
       </c>
       <c r="H71" t="s">
         <v>15</v>
@@ -3857,7 +3857,7 @@
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C72" t="s">
         <v>122</v>
@@ -3872,7 +3872,7 @@
         <v>14</v>
       </c>
       <c r="G72">
-        <v>11.44</v>
+        <v>13.25</v>
       </c>
       <c r="H72" t="s">
         <v>15</v>
@@ -3886,7 +3886,7 @@
         <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C73" t="s">
         <v>122</v>
@@ -3901,7 +3901,7 @@
         <v>14</v>
       </c>
       <c r="G73">
-        <v>13.25</v>
+        <v>13.05</v>
       </c>
       <c r="H73" t="s">
         <v>15</v>
@@ -3915,10 +3915,10 @@
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
@@ -3930,7 +3930,7 @@
         <v>14</v>
       </c>
       <c r="G74">
-        <v>13.05</v>
+        <v>13.96</v>
       </c>
       <c r="H74" t="s">
         <v>15</v>
@@ -3944,10 +3944,10 @@
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C75" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
@@ -3959,7 +3959,7 @@
         <v>14</v>
       </c>
       <c r="G75">
-        <v>13.96</v>
+        <v>13.88</v>
       </c>
       <c r="H75" t="s">
         <v>15</v>
@@ -3973,10 +3973,10 @@
         <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
@@ -3988,7 +3988,7 @@
         <v>14</v>
       </c>
       <c r="G76">
-        <v>13.88</v>
+        <v>13.99</v>
       </c>
       <c r="H76" t="s">
         <v>15</v>
@@ -4002,10 +4002,10 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -4017,7 +4017,7 @@
         <v>14</v>
       </c>
       <c r="G77">
-        <v>13.99</v>
+        <v>13.94</v>
       </c>
       <c r="H77" t="s">
         <v>15</v>
@@ -4031,10 +4031,10 @@
         <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
@@ -4060,10 +4060,10 @@
         <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C79" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -4075,7 +4075,7 @@
         <v>14</v>
       </c>
       <c r="G79">
-        <v>13.94</v>
+        <v>13.37</v>
       </c>
       <c r="H79" t="s">
         <v>15</v>
@@ -4089,7 +4089,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s">
         <v>136</v>
@@ -4104,7 +4104,7 @@
         <v>14</v>
       </c>
       <c r="G80">
-        <v>13.37</v>
+        <v>13.11</v>
       </c>
       <c r="H80" t="s">
         <v>15</v>
@@ -4118,10 +4118,10 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
@@ -4133,7 +4133,7 @@
         <v>14</v>
       </c>
       <c r="G81">
-        <v>13.11</v>
+        <v>12.5</v>
       </c>
       <c r="H81" t="s">
         <v>15</v>
@@ -4147,7 +4147,7 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C82" t="s">
         <v>139</v>
@@ -4162,7 +4162,7 @@
         <v>14</v>
       </c>
       <c r="G82">
-        <v>12.5</v>
+        <v>10.79</v>
       </c>
       <c r="H82" t="s">
         <v>15</v>
@@ -4176,7 +4176,7 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C83" t="s">
         <v>139</v>
@@ -4191,7 +4191,7 @@
         <v>14</v>
       </c>
       <c r="G83">
-        <v>10.79</v>
+        <v>11.83</v>
       </c>
       <c r="H83" t="s">
         <v>15</v>
@@ -4205,7 +4205,7 @@
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
         <v>139</v>
@@ -4220,7 +4220,7 @@
         <v>14</v>
       </c>
       <c r="G84">
-        <v>11.83</v>
+        <v>11.2</v>
       </c>
       <c r="H84" t="s">
         <v>15</v>
@@ -4234,7 +4234,7 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C85" t="s">
         <v>139</v>
@@ -4249,7 +4249,7 @@
         <v>14</v>
       </c>
       <c r="G85">
-        <v>11.2</v>
+        <v>9.98</v>
       </c>
       <c r="H85" t="s">
         <v>15</v>
@@ -4263,7 +4263,7 @@
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="C86" t="s">
         <v>139</v>
@@ -4278,7 +4278,7 @@
         <v>14</v>
       </c>
       <c r="G86">
-        <v>9.98</v>
+        <v>12.65</v>
       </c>
       <c r="H86" t="s">
         <v>15</v>
@@ -4292,10 +4292,10 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="C87" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
@@ -4307,7 +4307,7 @@
         <v>14</v>
       </c>
       <c r="G87">
-        <v>12.65</v>
+        <v>13.96</v>
       </c>
       <c r="H87" t="s">
         <v>15</v>
@@ -4321,10 +4321,10 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C88" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -4336,7 +4336,7 @@
         <v>14</v>
       </c>
       <c r="G88">
-        <v>13.96</v>
+        <v>13.83</v>
       </c>
       <c r="H88" t="s">
         <v>15</v>
@@ -4350,10 +4350,10 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="C89" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
@@ -4365,7 +4365,7 @@
         <v>14</v>
       </c>
       <c r="G89">
-        <v>13.83</v>
+        <v>11.64</v>
       </c>
       <c r="H89" t="s">
         <v>15</v>
@@ -4379,10 +4379,10 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="C90" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D90" t="s">
         <v>12</v>
@@ -4394,7 +4394,7 @@
         <v>14</v>
       </c>
       <c r="G90">
-        <v>11.64</v>
+        <v>13.8</v>
       </c>
       <c r="H90" t="s">
         <v>15</v>
@@ -4408,10 +4408,10 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C91" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
@@ -4423,7 +4423,7 @@
         <v>14</v>
       </c>
       <c r="G91">
-        <v>13.8</v>
+        <v>13.47</v>
       </c>
       <c r="H91" t="s">
         <v>15</v>
@@ -4437,10 +4437,10 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C92" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -4452,7 +4452,7 @@
         <v>14</v>
       </c>
       <c r="G92">
-        <v>13.47</v>
+        <v>13.59</v>
       </c>
       <c r="H92" t="s">
         <v>15</v>
@@ -4466,10 +4466,10 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C93" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
@@ -4481,7 +4481,7 @@
         <v>14</v>
       </c>
       <c r="G93">
-        <v>13.59</v>
+        <v>13.86</v>
       </c>
       <c r="H93" t="s">
         <v>15</v>
@@ -4495,10 +4495,10 @@
         <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C94" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D94" t="s">
         <v>12</v>
@@ -4510,7 +4510,7 @@
         <v>14</v>
       </c>
       <c r="G94">
-        <v>13.86</v>
+        <v>13.81</v>
       </c>
       <c r="H94" t="s">
         <v>15</v>
@@ -4524,10 +4524,10 @@
         <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C95" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D95" t="s">
         <v>12</v>
@@ -4539,7 +4539,7 @@
         <v>14</v>
       </c>
       <c r="G95">
-        <v>13.81</v>
+        <v>13.49</v>
       </c>
       <c r="H95" t="s">
         <v>15</v>
@@ -4553,10 +4553,10 @@
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C96" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D96" t="s">
         <v>12</v>
@@ -4568,7 +4568,7 @@
         <v>14</v>
       </c>
       <c r="G96">
-        <v>13.49</v>
+        <v>13.62</v>
       </c>
       <c r="H96" t="s">
         <v>15</v>
@@ -4582,7 +4582,7 @@
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s">
         <v>160</v>
@@ -4597,7 +4597,7 @@
         <v>14</v>
       </c>
       <c r="G97">
-        <v>13.62</v>
+        <v>12.96</v>
       </c>
       <c r="H97" t="s">
         <v>15</v>
@@ -4611,10 +4611,10 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C98" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D98" t="s">
         <v>12</v>
@@ -4626,7 +4626,7 @@
         <v>14</v>
       </c>
       <c r="G98">
-        <v>12.96</v>
+        <v>13.99</v>
       </c>
       <c r="H98" t="s">
         <v>15</v>
@@ -4640,10 +4640,10 @@
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
@@ -4655,7 +4655,7 @@
         <v>14</v>
       </c>
       <c r="G99">
-        <v>13.99</v>
+        <v>13.98</v>
       </c>
       <c r="H99" t="s">
         <v>15</v>
@@ -4669,10 +4669,10 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C100" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
@@ -4684,7 +4684,7 @@
         <v>14</v>
       </c>
       <c r="G100">
-        <v>13.98</v>
+        <v>13.96</v>
       </c>
       <c r="H100" t="s">
         <v>15</v>
@@ -4698,10 +4698,10 @@
         <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C101" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
@@ -4727,10 +4727,10 @@
         <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C102" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
@@ -4742,7 +4742,7 @@
         <v>14</v>
       </c>
       <c r="G102">
-        <v>13.96</v>
+        <v>11.755000000000001</v>
       </c>
       <c r="H102" t="s">
         <v>15</v>
@@ -4756,7 +4756,7 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C103" t="s">
         <v>169</v>
@@ -4771,7 +4771,7 @@
         <v>14</v>
       </c>
       <c r="G103">
-        <v>11.755000000000001</v>
+        <v>10.43</v>
       </c>
       <c r="H103" t="s">
         <v>15</v>
@@ -4785,10 +4785,10 @@
         <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C104" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D104" t="s">
         <v>12</v>
@@ -4800,7 +4800,7 @@
         <v>14</v>
       </c>
       <c r="G104">
-        <v>10.43</v>
+        <v>13.55</v>
       </c>
       <c r="H104" t="s">
         <v>15</v>
@@ -4814,10 +4814,10 @@
         <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C105" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D105" t="s">
         <v>12</v>
@@ -4829,7 +4829,7 @@
         <v>14</v>
       </c>
       <c r="G105">
-        <v>13.55</v>
+        <v>13.08</v>
       </c>
       <c r="H105" t="s">
         <v>15</v>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C106" t="s">
         <v>174</v>
@@ -4858,7 +4858,7 @@
         <v>14</v>
       </c>
       <c r="G106">
-        <v>13.08</v>
+        <v>10.67</v>
       </c>
       <c r="H106" t="s">
         <v>15</v>
@@ -4872,7 +4872,7 @@
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C107" t="s">
         <v>174</v>
@@ -4887,7 +4887,7 @@
         <v>14</v>
       </c>
       <c r="G107">
-        <v>10.67</v>
+        <v>12.24</v>
       </c>
       <c r="H107" t="s">
         <v>15</v>
@@ -4901,7 +4901,7 @@
         <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C108" t="s">
         <v>174</v>
@@ -4916,7 +4916,7 @@
         <v>14</v>
       </c>
       <c r="G108">
-        <v>12.24</v>
+        <v>11.99</v>
       </c>
       <c r="H108" t="s">
         <v>15</v>
@@ -4930,7 +4930,7 @@
         <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C109" t="s">
         <v>174</v>
@@ -4945,7 +4945,7 @@
         <v>14</v>
       </c>
       <c r="G109">
-        <v>11.99</v>
+        <v>10.72</v>
       </c>
       <c r="H109" t="s">
         <v>15</v>
@@ -4959,7 +4959,7 @@
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>178</v>
+        <v>64</v>
       </c>
       <c r="C110" t="s">
         <v>174</v>
@@ -4974,7 +4974,7 @@
         <v>14</v>
       </c>
       <c r="G110">
-        <v>10.72</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="H110" t="s">
         <v>15</v>
@@ -4988,10 +4988,10 @@
         <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
       <c r="C111" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D111" t="s">
         <v>12</v>
@@ -5003,7 +5003,7 @@
         <v>14</v>
       </c>
       <c r="G111">
-        <v>9.5399999999999991</v>
+        <v>13.25</v>
       </c>
       <c r="H111" t="s">
         <v>15</v>
@@ -5017,7 +5017,7 @@
         <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C112" t="s">
         <v>180</v>
@@ -5032,7 +5032,7 @@
         <v>14</v>
       </c>
       <c r="G112">
-        <v>13.25</v>
+        <v>13.29</v>
       </c>
       <c r="H112" t="s">
         <v>15</v>
@@ -5046,10 +5046,10 @@
         <v>9</v>
       </c>
       <c r="B113" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -5061,7 +5061,7 @@
         <v>14</v>
       </c>
       <c r="G113">
-        <v>13.29</v>
+        <v>12.24</v>
       </c>
       <c r="H113" t="s">
         <v>15</v>
@@ -5075,7 +5075,7 @@
         <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C114" t="s">
         <v>183</v>
@@ -5090,7 +5090,7 @@
         <v>14</v>
       </c>
       <c r="G114">
-        <v>12.24</v>
+        <v>9.4</v>
       </c>
       <c r="H114" t="s">
         <v>15</v>
@@ -5104,7 +5104,7 @@
         <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C115" t="s">
         <v>183</v>
@@ -5119,7 +5119,7 @@
         <v>14</v>
       </c>
       <c r="G115">
-        <v>9.4</v>
+        <v>13.47</v>
       </c>
       <c r="H115" t="s">
         <v>15</v>
@@ -5133,7 +5133,7 @@
         <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C116" t="s">
         <v>183</v>
@@ -5148,7 +5148,7 @@
         <v>14</v>
       </c>
       <c r="G116">
-        <v>13.47</v>
+        <v>10.76</v>
       </c>
       <c r="H116" t="s">
         <v>15</v>
@@ -5162,7 +5162,7 @@
         <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C117" t="s">
         <v>183</v>
@@ -5177,7 +5177,7 @@
         <v>14</v>
       </c>
       <c r="G117">
-        <v>10.76</v>
+        <v>12.88</v>
       </c>
       <c r="H117" t="s">
         <v>15</v>
@@ -5191,10 +5191,10 @@
         <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C118" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
@@ -5206,7 +5206,7 @@
         <v>14</v>
       </c>
       <c r="G118">
-        <v>12.88</v>
+        <v>8.02</v>
       </c>
       <c r="H118" t="s">
         <v>15</v>
@@ -5220,7 +5220,7 @@
         <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C119" t="s">
         <v>189</v>
@@ -5235,7 +5235,7 @@
         <v>14</v>
       </c>
       <c r="G119">
-        <v>8.02</v>
+        <v>11.71</v>
       </c>
       <c r="H119" t="s">
         <v>15</v>
@@ -5249,7 +5249,7 @@
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C120" t="s">
         <v>189</v>
@@ -5264,7 +5264,7 @@
         <v>14</v>
       </c>
       <c r="G120">
-        <v>11.71</v>
+        <v>10.35</v>
       </c>
       <c r="H120" t="s">
         <v>15</v>
@@ -5278,7 +5278,7 @@
         <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C121" t="s">
         <v>189</v>
@@ -5293,7 +5293,7 @@
         <v>14</v>
       </c>
       <c r="G121">
-        <v>10.35</v>
+        <v>11.99</v>
       </c>
       <c r="H121" t="s">
         <v>15</v>
@@ -5307,7 +5307,7 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C122" t="s">
         <v>189</v>
@@ -5322,7 +5322,7 @@
         <v>14</v>
       </c>
       <c r="G122">
-        <v>11.99</v>
+        <v>10.23</v>
       </c>
       <c r="H122" t="s">
         <v>15</v>
@@ -5336,7 +5336,7 @@
         <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C123" t="s">
         <v>189</v>
@@ -5351,7 +5351,7 @@
         <v>14</v>
       </c>
       <c r="G123">
-        <v>10.23</v>
+        <v>13.36</v>
       </c>
       <c r="H123" t="s">
         <v>15</v>
@@ -5365,7 +5365,7 @@
         <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C124" t="s">
         <v>189</v>
@@ -5380,7 +5380,7 @@
         <v>14</v>
       </c>
       <c r="G124">
-        <v>13.36</v>
+        <v>11.9</v>
       </c>
       <c r="H124" t="s">
         <v>15</v>
@@ -5394,10 +5394,10 @@
         <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C125" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D125" t="s">
         <v>12</v>
@@ -5409,7 +5409,7 @@
         <v>14</v>
       </c>
       <c r="G125">
-        <v>11.9</v>
+        <v>13.24</v>
       </c>
       <c r="H125" t="s">
         <v>15</v>
@@ -5423,7 +5423,7 @@
         <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C126" t="s">
         <v>197</v>
@@ -5438,7 +5438,7 @@
         <v>14</v>
       </c>
       <c r="G126">
-        <v>13.24</v>
+        <v>10.52</v>
       </c>
       <c r="H126" t="s">
         <v>15</v>
@@ -5452,10 +5452,10 @@
         <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C127" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -5467,7 +5467,7 @@
         <v>14</v>
       </c>
       <c r="G127">
-        <v>10.52</v>
+        <v>13.99</v>
       </c>
       <c r="H127" t="s">
         <v>15</v>
@@ -5481,10 +5481,10 @@
         <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>198</v>
+        <v>35</v>
       </c>
       <c r="C128" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
@@ -5496,7 +5496,7 @@
         <v>14</v>
       </c>
       <c r="G128">
-        <v>13.99</v>
+        <v>13.3</v>
       </c>
       <c r="H128" t="s">
         <v>15</v>
@@ -5510,7 +5510,7 @@
         <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>35</v>
+        <v>201</v>
       </c>
       <c r="C129" t="s">
         <v>200</v>
@@ -5525,7 +5525,7 @@
         <v>14</v>
       </c>
       <c r="G129">
-        <v>13.3</v>
+        <v>13.31</v>
       </c>
       <c r="H129" t="s">
         <v>15</v>
@@ -5539,10 +5539,10 @@
         <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C130" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
@@ -5554,7 +5554,7 @@
         <v>14</v>
       </c>
       <c r="G130">
-        <v>13.31</v>
+        <v>13.38</v>
       </c>
       <c r="H130" t="s">
         <v>15</v>
@@ -5568,10 +5568,10 @@
         <v>9</v>
       </c>
       <c r="B131" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C131" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
@@ -5583,7 +5583,7 @@
         <v>14</v>
       </c>
       <c r="G131">
-        <v>13.38</v>
+        <v>13.16</v>
       </c>
       <c r="H131" t="s">
         <v>15</v>
@@ -5597,7 +5597,7 @@
         <v>9</v>
       </c>
       <c r="B132" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C132" t="s">
         <v>205</v>
@@ -5612,7 +5612,7 @@
         <v>14</v>
       </c>
       <c r="G132">
-        <v>13.16</v>
+        <v>13.11</v>
       </c>
       <c r="H132" t="s">
         <v>15</v>
@@ -5626,10 +5626,10 @@
         <v>9</v>
       </c>
       <c r="B133" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C133" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D133" t="s">
         <v>12</v>
@@ -5641,7 +5641,7 @@
         <v>14</v>
       </c>
       <c r="G133">
-        <v>13.11</v>
+        <v>13.96</v>
       </c>
       <c r="H133" t="s">
         <v>15</v>
@@ -5655,10 +5655,10 @@
         <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C134" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D134" t="s">
         <v>12</v>
@@ -5670,7 +5670,7 @@
         <v>14</v>
       </c>
       <c r="G134">
-        <v>13.96</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="H134" t="s">
         <v>15</v>
@@ -5684,7 +5684,7 @@
         <v>9</v>
       </c>
       <c r="B135" t="s">
-        <v>209</v>
+        <v>108</v>
       </c>
       <c r="C135" t="s">
         <v>210</v>
@@ -5699,7 +5699,7 @@
         <v>14</v>
       </c>
       <c r="G135">
-        <v>10.199999999999999</v>
+        <v>12.65</v>
       </c>
       <c r="H135" t="s">
         <v>15</v>
@@ -5713,7 +5713,7 @@
         <v>9</v>
       </c>
       <c r="B136" t="s">
-        <v>108</v>
+        <v>211</v>
       </c>
       <c r="C136" t="s">
         <v>210</v>
@@ -5728,7 +5728,7 @@
         <v>14</v>
       </c>
       <c r="G136">
-        <v>12.65</v>
+        <v>12.58</v>
       </c>
       <c r="H136" t="s">
         <v>15</v>
@@ -5742,10 +5742,10 @@
         <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="C137" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
@@ -5757,7 +5757,7 @@
         <v>14</v>
       </c>
       <c r="G137">
-        <v>12.58</v>
+        <v>13.36</v>
       </c>
       <c r="H137" t="s">
         <v>15</v>
@@ -5767,23 +5767,11 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>9</v>
-      </c>
       <c r="B138" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="C138" t="s">
-        <v>49</v>
-      </c>
-      <c r="D138" t="s">
-        <v>12</v>
-      </c>
-      <c r="E138" t="s">
-        <v>13</v>
-      </c>
-      <c r="F138" t="s">
-        <v>14</v>
+        <v>213</v>
       </c>
       <c r="G138">
         <v>13.36</v>
@@ -5792,18 +5780,18 @@
         <v>15</v>
       </c>
       <c r="I138" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C139" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G139">
-        <v>13.36</v>
+        <v>13.94</v>
       </c>
       <c r="H139" t="s">
         <v>15</v>
@@ -5814,13 +5802,13 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C140" t="s">
-        <v>216</v>
+        <v>95</v>
       </c>
       <c r="G140">
-        <v>13.94</v>
+        <v>13.05</v>
       </c>
       <c r="H140" t="s">
         <v>15</v>
@@ -5831,13 +5819,13 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C141" t="s">
-        <v>95</v>
+        <v>219</v>
       </c>
       <c r="G141">
-        <v>13.05</v>
+        <v>13.88</v>
       </c>
       <c r="H141" t="s">
         <v>15</v>
@@ -5848,13 +5836,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C142" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G142">
-        <v>13.88</v>
+        <v>12.705</v>
       </c>
       <c r="H142" t="s">
         <v>15</v>
@@ -5865,13 +5853,13 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C143" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="G143">
-        <v>12.705</v>
+        <v>10.08</v>
       </c>
       <c r="H143" t="s">
         <v>15</v>
@@ -5882,13 +5870,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C144" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="G144">
-        <v>10.08</v>
+        <v>11.99</v>
       </c>
       <c r="H144" t="s">
         <v>15</v>
@@ -5899,13 +5887,13 @@
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="C145" t="s">
-        <v>139</v>
+        <v>224</v>
       </c>
       <c r="G145">
-        <v>11.99</v>
+        <v>12.61</v>
       </c>
       <c r="H145" t="s">
         <v>15</v>
@@ -5916,13 +5904,13 @@
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="C146" t="s">
         <v>224</v>
       </c>
       <c r="G146">
-        <v>12.61</v>
+        <v>12.62</v>
       </c>
       <c r="H146" t="s">
         <v>15</v>
@@ -5933,7 +5921,7 @@
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="C147" t="s">
         <v>224</v>
@@ -5950,13 +5938,13 @@
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="C148" t="s">
         <v>224</v>
       </c>
       <c r="G148">
-        <v>12.62</v>
+        <v>12.6</v>
       </c>
       <c r="H148" t="s">
         <v>15</v>
@@ -5967,13 +5955,13 @@
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="C149" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G149">
-        <v>12.6</v>
+        <v>13.88</v>
       </c>
       <c r="H149" t="s">
         <v>15</v>
@@ -5984,13 +5972,13 @@
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C150" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G150">
-        <v>13.88</v>
+        <v>13.69</v>
       </c>
       <c r="H150" t="s">
         <v>15</v>
@@ -6001,13 +5989,13 @@
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C151" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G151">
-        <v>13.69</v>
+        <v>13.31</v>
       </c>
       <c r="H151" t="s">
         <v>15</v>
@@ -6018,13 +6006,13 @@
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C152" t="s">
-        <v>230</v>
+        <v>169</v>
       </c>
       <c r="G152">
-        <v>13.31</v>
+        <v>10.105</v>
       </c>
       <c r="H152" t="s">
         <v>15</v>
@@ -6035,13 +6023,13 @@
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C153" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="G153">
-        <v>10.105</v>
+        <v>13.99</v>
       </c>
       <c r="H153" t="s">
         <v>15</v>
@@ -6052,13 +6040,13 @@
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C154" t="s">
-        <v>232</v>
+        <v>151</v>
       </c>
       <c r="G154">
-        <v>13.99</v>
+        <v>13.18</v>
       </c>
       <c r="H154" t="s">
         <v>15</v>
@@ -6069,13 +6057,13 @@
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C155" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="G155">
-        <v>13.18</v>
+        <v>13.14</v>
       </c>
       <c r="H155" t="s">
         <v>15</v>
@@ -6086,13 +6074,13 @@
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C156" t="s">
         <v>235</v>
       </c>
       <c r="G156">
-        <v>13.14</v>
+        <v>13</v>
       </c>
       <c r="H156" t="s">
         <v>15</v>
@@ -6103,13 +6091,13 @@
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C157" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G157">
-        <v>13</v>
+        <v>13.37</v>
       </c>
       <c r="H157" t="s">
         <v>15</v>
@@ -6120,13 +6108,13 @@
     </row>
     <row r="158" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="C158" t="s">
-        <v>238</v>
+        <v>105</v>
       </c>
       <c r="G158">
-        <v>13.37</v>
+        <v>12.1</v>
       </c>
       <c r="H158" t="s">
         <v>15</v>
@@ -6137,13 +6125,13 @@
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="C159" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="G159">
-        <v>12.1</v>
+        <v>13.97</v>
       </c>
       <c r="H159" t="s">
         <v>15</v>
@@ -6154,13 +6142,13 @@
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C160" t="s">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="G160">
-        <v>13.97</v>
+        <v>12.46</v>
       </c>
       <c r="H160" t="s">
         <v>15</v>
@@ -6171,13 +6159,13 @@
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C161" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="G161">
-        <v>12.46</v>
+        <v>11.98</v>
       </c>
       <c r="H161" t="s">
         <v>15</v>
@@ -6188,13 +6176,13 @@
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C162" t="s">
-        <v>136</v>
+        <v>244</v>
       </c>
       <c r="G162">
-        <v>11.98</v>
+        <v>13.88</v>
       </c>
       <c r="H162" t="s">
         <v>15</v>
@@ -6205,13 +6193,13 @@
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C163" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G163">
-        <v>13.88</v>
+        <v>13.27</v>
       </c>
       <c r="H163" t="s">
         <v>15</v>
@@ -6222,7 +6210,7 @@
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C164" t="s">
         <v>246</v>
@@ -6239,13 +6227,13 @@
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C165" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G165">
-        <v>13.27</v>
+        <v>13.99</v>
       </c>
       <c r="H165" t="s">
         <v>15</v>
@@ -6256,13 +6244,13 @@
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C166" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G166">
-        <v>13.99</v>
+        <v>13.93</v>
       </c>
       <c r="H166" t="s">
         <v>15</v>
@@ -6273,13 +6261,13 @@
     </row>
     <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="C167" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G167">
-        <v>13.93</v>
+        <v>9.67</v>
       </c>
       <c r="H167" t="s">
         <v>15</v>
@@ -6290,13 +6278,13 @@
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>194</v>
+        <v>253</v>
       </c>
       <c r="C168" t="s">
-        <v>252</v>
+        <v>189</v>
       </c>
       <c r="G168">
-        <v>9.67</v>
+        <v>9.49</v>
       </c>
       <c r="H168" t="s">
         <v>15</v>
@@ -6307,13 +6295,13 @@
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C169" t="s">
-        <v>189</v>
+        <v>255</v>
       </c>
       <c r="G169">
-        <v>9.49</v>
+        <v>13.99</v>
       </c>
       <c r="H169" t="s">
         <v>15</v>
@@ -6324,13 +6312,13 @@
     </row>
     <row r="170" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C170" t="s">
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="G170">
-        <v>13.99</v>
+        <v>11.48</v>
       </c>
       <c r="H170" t="s">
         <v>15</v>
@@ -6341,13 +6329,13 @@
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C171" t="s">
         <v>180</v>
       </c>
       <c r="G171">
-        <v>11.48</v>
+        <v>8.35</v>
       </c>
       <c r="H171" t="s">
         <v>15</v>
@@ -6358,13 +6346,13 @@
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C172" t="s">
-        <v>180</v>
+        <v>259</v>
       </c>
       <c r="G172">
-        <v>8.35</v>
+        <v>13.99</v>
       </c>
       <c r="H172" t="s">
         <v>15</v>
@@ -6375,13 +6363,13 @@
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>258</v>
+        <v>101</v>
       </c>
       <c r="C173" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G173">
-        <v>13.99</v>
+        <v>12.71</v>
       </c>
       <c r="H173" t="s">
         <v>15</v>
@@ -6392,35 +6380,18 @@
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>101</v>
+        <v>261</v>
       </c>
       <c r="C174" t="s">
         <v>260</v>
       </c>
       <c r="G174">
-        <v>12.71</v>
+        <v>13.23</v>
       </c>
       <c r="H174" t="s">
         <v>15</v>
       </c>
       <c r="I174" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>261</v>
-      </c>
-      <c r="C175" t="s">
-        <v>260</v>
-      </c>
-      <c r="G175">
-        <v>13.23</v>
-      </c>
-      <c r="H175" t="s">
-        <v>15</v>
-      </c>
-      <c r="I175" t="s">
         <v>214</v>
       </c>
     </row>
@@ -6430,11 +6401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="A1:D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>